<commit_message>
scenequest can work now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SceneQuest.xlsx
+++ b/ConfigData/Xlsx/SceneQuest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\用户目录\我的文档\FEWin\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2757,14 +2757,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>kil;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>kil;1;kin;1;wat;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>hiddeway</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3142,6 +3134,14 @@
   </si>
   <si>
     <t>baludi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kil+;kin-;wat+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kil+</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6355,8 +6355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6415,7 +6415,7 @@
         <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>619</v>
@@ -6538,7 +6538,7 @@
         <v>69</v>
       </c>
       <c r="AX1" s="88" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="AY1" s="88" t="s">
         <v>630</v>
@@ -6607,10 +6607,10 @@
         <v>332</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.15">
@@ -6863,7 +6863,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="80" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="J3" s="80" t="s">
         <v>621</v>
@@ -7055,10 +7055,10 @@
         <v>334</v>
       </c>
       <c r="BU3" s="80" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="BV3" s="80" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.15">
@@ -7075,7 +7075,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="70" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>30</v>
@@ -7093,10 +7093,10 @@
       <c r="R4" s="100"/>
       <c r="S4" s="22"/>
       <c r="T4" s="67" t="s">
-        <v>675</v>
+        <v>775</v>
       </c>
       <c r="U4" s="67" t="s">
-        <v>676</v>
+        <v>774</v>
       </c>
       <c r="V4" s="70" t="s">
         <v>670</v>
@@ -7194,10 +7194,10 @@
         <v>35</v>
       </c>
       <c r="BU4" s="70" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="BV4" s="70" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="5" spans="1:74" x14ac:dyDescent="0.15">
@@ -7263,7 +7263,7 @@
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="26" t="s">
@@ -7309,7 +7309,7 @@
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="26" t="s">
@@ -7355,7 +7355,7 @@
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="26" t="s">
@@ -7403,10 +7403,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="70" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G9" s="70" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="67"/>
@@ -7453,11 +7453,11 @@
         <v>473</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="27" t="s">
@@ -7766,7 +7766,7 @@
         <v>42000015</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
@@ -7778,14 +7778,14 @@
         <v>1</v>
       </c>
       <c r="F16" s="70" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G16" s="70" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J16" s="103"/>
       <c r="K16" s="30" t="s">
@@ -7803,7 +7803,7 @@
       <c r="U16" s="67"/>
       <c r="V16" s="67"/>
       <c r="W16" s="66" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="X16" s="22" t="s">
         <v>11</v>
@@ -7812,7 +7812,7 @@
         <v>100</v>
       </c>
       <c r="AZ16" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA16" s="8">
         <v>1</v>
@@ -7824,10 +7824,10 @@
         <v>200</v>
       </c>
       <c r="BU16" s="70" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="BV16" s="70" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="17" spans="1:74" x14ac:dyDescent="0.15">
@@ -7835,7 +7835,7 @@
         <v>42000016</v>
       </c>
       <c r="B17" s="71" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
@@ -7847,14 +7847,14 @@
         <v>2</v>
       </c>
       <c r="F17" s="70" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G17" s="70" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J17" s="103"/>
       <c r="K17" s="30" t="s">
@@ -7872,14 +7872,14 @@
       <c r="U17" s="67"/>
       <c r="V17" s="67"/>
       <c r="W17" s="66" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="X17" s="22"/>
       <c r="AQ17" s="8">
         <v>100</v>
       </c>
       <c r="AZ17" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA17" s="8">
         <v>1</v>
@@ -7891,10 +7891,10 @@
         <v>400</v>
       </c>
       <c r="BU17" s="70" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="BV17" s="70" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="18" spans="1:74" x14ac:dyDescent="0.15">
@@ -7983,7 +7983,7 @@
       <c r="W19" s="24"/>
       <c r="X19" s="22"/>
       <c r="BU19" s="70" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="BV19" s="70" t="s">
         <v>213</v>
@@ -8072,7 +8072,7 @@
       <c r="S21" s="22"/>
       <c r="T21" s="22"/>
       <c r="U21" s="22" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V21" s="22"/>
       <c r="W21" s="24"/>
@@ -8125,7 +8125,7 @@
       <c r="S22" s="22"/>
       <c r="T22" s="22"/>
       <c r="U22" s="67" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="V22" s="67"/>
       <c r="X22" s="22"/>
@@ -8222,7 +8222,7 @@
       <c r="S24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="67" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="V24" s="67"/>
       <c r="W24" s="23"/>
@@ -8272,7 +8272,7 @@
       <c r="S25" s="22"/>
       <c r="T25" s="22"/>
       <c r="U25" s="67" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="V25" s="67"/>
       <c r="W25" s="23"/>
@@ -8355,14 +8355,14 @@
         <v>1</v>
       </c>
       <c r="F27" s="70" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="30" t="s">
@@ -8378,7 +8378,7 @@
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
       <c r="U27" s="67" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="V27" s="22"/>
       <c r="W27" s="24" t="s">
@@ -8394,7 +8394,7 @@
         <v>100</v>
       </c>
       <c r="AZ27" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA27" s="8">
         <v>1</v>
@@ -8432,14 +8432,14 @@
         <v>1</v>
       </c>
       <c r="F28" s="70" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G28" s="70" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="30" t="s">
@@ -8455,10 +8455,10 @@
       <c r="S28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="67" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="V28" s="67" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="W28" s="24" t="s">
         <v>296</v>
@@ -8473,7 +8473,7 @@
         <v>50</v>
       </c>
       <c r="AZ28" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA28" s="8">
         <v>1</v>
@@ -8532,7 +8532,7 @@
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
       <c r="U29" s="67" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="V29" s="67"/>
       <c r="W29" s="24"/>
@@ -8577,14 +8577,14 @@
         <v>1</v>
       </c>
       <c r="F30" s="70" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="G30" s="70" t="s">
         <v>166</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J30" s="22"/>
       <c r="K30" s="30" t="s">
@@ -8614,7 +8614,7 @@
         <v>100</v>
       </c>
       <c r="AZ30" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA30" s="8">
         <v>1</v>
@@ -8652,14 +8652,14 @@
         <v>1</v>
       </c>
       <c r="F31" s="70" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G31" s="70" t="s">
         <v>528</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J31" s="22"/>
       <c r="K31" s="79" t="s">
@@ -8689,7 +8689,7 @@
         <v>150</v>
       </c>
       <c r="AZ31" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA31" s="8">
         <v>1</v>
@@ -8734,7 +8734,7 @@
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="67" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J32" s="22"/>
       <c r="K32" s="30" t="s">
@@ -8750,7 +8750,7 @@
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="67" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="V32" s="67"/>
       <c r="W32" s="24" t="s">
@@ -8769,7 +8769,7 @@
         <v>362</v>
       </c>
       <c r="AZ32" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA32" s="8">
         <v>1</v>
@@ -8831,7 +8831,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
       <c r="U33" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V33" s="67"/>
       <c r="X33" s="22"/>
@@ -8941,12 +8941,12 @@
       <c r="T35" s="22"/>
       <c r="U35" s="22"/>
       <c r="V35" s="67" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="W35" s="24"/>
       <c r="X35" s="22"/>
       <c r="BU35" s="70" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BV35" s="70" t="s">
         <v>85</v>
@@ -8992,7 +8992,7 @@
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
       <c r="U36" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V36" s="67"/>
       <c r="W36" s="23"/>
@@ -9050,7 +9050,7 @@
       <c r="S37" s="22"/>
       <c r="T37" s="22"/>
       <c r="U37" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V37" s="67"/>
       <c r="X37" s="22"/>
@@ -9105,7 +9105,7 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
       <c r="U38" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V38" s="67"/>
       <c r="W38" s="24"/>
@@ -9137,14 +9137,14 @@
         <v>2</v>
       </c>
       <c r="F39" s="70" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>144</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J39" s="22"/>
       <c r="K39" s="30" t="s">
@@ -9160,7 +9160,7 @@
       <c r="S39" s="22"/>
       <c r="T39" s="22"/>
       <c r="U39" s="67" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="V39" s="67"/>
       <c r="W39" s="24" t="s">
@@ -9176,7 +9176,7 @@
         <v>271</v>
       </c>
       <c r="AZ39" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA39" s="8">
         <v>1</v>
@@ -9229,7 +9229,7 @@
       <c r="S40" s="22"/>
       <c r="T40" s="22"/>
       <c r="U40" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V40" s="67"/>
       <c r="W40" s="24"/>
@@ -9431,7 +9431,7 @@
       <c r="S44" s="22"/>
       <c r="T44" s="22"/>
       <c r="U44" s="67" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="V44" s="67"/>
       <c r="W44" s="23"/>
@@ -9529,14 +9529,14 @@
         <v>1</v>
       </c>
       <c r="F46" s="70" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>257</v>
       </c>
       <c r="H46" s="22"/>
       <c r="I46" s="67" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="J46" s="22"/>
       <c r="K46" s="30" t="s">
@@ -9552,7 +9552,7 @@
       <c r="S46" s="22"/>
       <c r="T46" s="22"/>
       <c r="U46" s="22" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="V46" s="22"/>
       <c r="W46" s="24" t="s">
@@ -9568,7 +9568,7 @@
         <v>50</v>
       </c>
       <c r="AZ46" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA46" s="8">
         <v>1</v>
@@ -9603,14 +9603,14 @@
         <v>2</v>
       </c>
       <c r="F47" s="70" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>451</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J47" s="22"/>
       <c r="K47" s="30" t="s">
@@ -9626,7 +9626,7 @@
       <c r="S47" s="22"/>
       <c r="T47" s="22"/>
       <c r="U47" s="67" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="V47" s="67"/>
       <c r="W47" s="23" t="s">
@@ -9642,7 +9642,7 @@
         <v>50</v>
       </c>
       <c r="AZ47" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA47" s="8">
         <v>1</v>
@@ -9684,7 +9684,7 @@
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="67" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J48" s="22"/>
       <c r="K48" s="29" t="s">
@@ -9722,7 +9722,7 @@
         <v>310</v>
       </c>
       <c r="AZ48" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA48" s="8">
         <v>1</v>
@@ -9829,14 +9829,14 @@
         <v>1</v>
       </c>
       <c r="F50" s="70" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>236</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="22" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J50" s="22"/>
       <c r="K50" s="30" t="s">
@@ -9852,7 +9852,7 @@
       <c r="S50" s="22"/>
       <c r="T50" s="22"/>
       <c r="U50" s="67" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="V50" s="67"/>
       <c r="W50" s="23" t="s">
@@ -9871,7 +9871,7 @@
         <v>100</v>
       </c>
       <c r="AZ50" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA50" s="8">
         <v>1</v>
@@ -10031,14 +10031,14 @@
         <v>2</v>
       </c>
       <c r="F53" s="70" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>340</v>
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J53" s="22"/>
       <c r="K53" s="30" t="s">
@@ -10054,7 +10054,7 @@
       <c r="S53" s="22"/>
       <c r="T53" s="22"/>
       <c r="U53" s="67" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="V53" s="67"/>
       <c r="W53" s="8" t="s">
@@ -10070,7 +10070,7 @@
         <v>50</v>
       </c>
       <c r="AZ53" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA53" s="8">
         <v>1</v>
@@ -10531,14 +10531,14 @@
         <v>2</v>
       </c>
       <c r="F61" s="70" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>415</v>
       </c>
       <c r="H61" s="22"/>
       <c r="I61" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J61" s="22"/>
       <c r="K61" s="30" t="s">
@@ -10554,7 +10554,7 @@
       <c r="S61" s="22"/>
       <c r="T61" s="22"/>
       <c r="U61" s="22" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="V61" s="22"/>
       <c r="W61" s="8" t="s">
@@ -10570,7 +10570,7 @@
         <v>70</v>
       </c>
       <c r="AZ61" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA61" s="8">
         <v>1</v>
@@ -10676,14 +10676,14 @@
         <v>2</v>
       </c>
       <c r="F63" s="70" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>443</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J63" s="22"/>
       <c r="K63" s="29" t="s">
@@ -10718,7 +10718,7 @@
         <v>446</v>
       </c>
       <c r="AZ63" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA63" s="8">
         <v>1</v>
@@ -10777,14 +10777,14 @@
         <v>2</v>
       </c>
       <c r="F64" s="70" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>455</v>
       </c>
       <c r="H64" s="22"/>
       <c r="I64" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J64" s="22"/>
       <c r="K64" s="29" t="s">
@@ -10822,7 +10822,7 @@
         <v>50</v>
       </c>
       <c r="AZ64" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA64" s="8">
         <v>1</v>
@@ -10997,14 +10997,14 @@
         <v>2</v>
       </c>
       <c r="F67" s="70" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G67" s="70" t="s">
         <v>536</v>
       </c>
       <c r="H67" s="67"/>
       <c r="I67" s="67" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J67" s="67"/>
       <c r="K67" s="30" t="s">
@@ -11141,7 +11141,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="70" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G69" s="8" t="s">
         <v>326</v>
@@ -11211,7 +11211,7 @@
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
       <c r="J70" s="103" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="K70" s="30" t="s">
         <v>228</v>
@@ -11227,10 +11227,10 @@
       </c>
       <c r="S70" s="22"/>
       <c r="T70" s="67" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="U70" s="67" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="V70" s="67"/>
       <c r="W70" s="23" t="s">
@@ -11294,10 +11294,10 @@
       </c>
       <c r="S71" s="22"/>
       <c r="T71" s="67" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="U71" s="67" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="V71" s="67"/>
       <c r="W71" s="24" t="s">
@@ -11376,10 +11376,10 @@
       </c>
       <c r="S72" s="22"/>
       <c r="T72" s="67" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="U72" s="67" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V72" s="67"/>
       <c r="W72" s="24"/>
@@ -11439,10 +11439,10 @@
       </c>
       <c r="S73" s="22"/>
       <c r="T73" s="67" t="s">
+        <v>696</v>
+      </c>
+      <c r="U73" s="67" t="s">
         <v>698</v>
-      </c>
-      <c r="U73" s="67" t="s">
-        <v>700</v>
       </c>
       <c r="V73" s="67"/>
       <c r="X73" s="22"/>
@@ -11503,10 +11503,10 @@
       </c>
       <c r="S74" s="22"/>
       <c r="T74" s="67" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="U74" s="67" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="V74" s="67"/>
       <c r="W74" s="24" t="s">
@@ -11582,10 +11582,10 @@
       </c>
       <c r="S75" s="22"/>
       <c r="T75" s="67" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="U75" s="67" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="V75" s="67"/>
       <c r="W75" s="24" t="s">
@@ -11692,10 +11692,10 @@
       </c>
       <c r="S77" s="22"/>
       <c r="T77" s="67" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="U77" s="67" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="V77" s="67"/>
       <c r="W77" s="24"/>
@@ -11761,10 +11761,10 @@
       </c>
       <c r="S78" s="22"/>
       <c r="T78" s="67" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="U78" s="67" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="V78" s="67"/>
       <c r="W78" s="24"/>
@@ -11828,10 +11828,10 @@
       </c>
       <c r="S79" s="22"/>
       <c r="T79" s="67" t="s">
+        <v>680</v>
+      </c>
+      <c r="U79" s="67" t="s">
         <v>682</v>
-      </c>
-      <c r="U79" s="67" t="s">
-        <v>684</v>
       </c>
       <c r="V79" s="67"/>
       <c r="X79" s="22"/>
@@ -11887,7 +11887,7 @@
       </c>
       <c r="S80" s="22"/>
       <c r="T80" s="67" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="U80" s="22"/>
       <c r="V80" s="22"/>
@@ -12070,7 +12070,7 @@
       </c>
       <c r="S83" s="22"/>
       <c r="T83" s="67" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="U83" s="22"/>
       <c r="V83" s="22"/>
@@ -12130,7 +12130,7 @@
       <c r="S84" s="22"/>
       <c r="T84" s="22"/>
       <c r="U84" s="22" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V84" s="22"/>
       <c r="W84" s="8" t="s">
@@ -12204,10 +12204,10 @@
       </c>
       <c r="S85" s="22"/>
       <c r="T85" s="67" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="U85" s="67" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="V85" s="67"/>
       <c r="X85" s="22"/>
@@ -12250,7 +12250,7 @@
       <c r="H86" s="22"/>
       <c r="I86" s="22"/>
       <c r="J86" s="67" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="K86" s="30" t="s">
         <v>228</v>
@@ -12266,10 +12266,10 @@
       </c>
       <c r="S86" s="22"/>
       <c r="T86" s="67" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="U86" s="67" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V86" s="67"/>
       <c r="W86" s="24" t="s">
@@ -12387,7 +12387,7 @@
       <c r="H88" s="22"/>
       <c r="I88" s="22"/>
       <c r="J88" s="67" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="K88" s="30" t="s">
         <v>228</v>
@@ -12403,10 +12403,10 @@
       </c>
       <c r="S88" s="22"/>
       <c r="T88" s="67" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="U88" s="67" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V88" s="67"/>
       <c r="W88" s="24" t="s">
@@ -12883,7 +12883,7 @@
       </c>
       <c r="H95" s="67"/>
       <c r="I95" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J95" s="67"/>
       <c r="K95" s="31" t="s">
@@ -12950,7 +12950,7 @@
       </c>
       <c r="H96" s="67"/>
       <c r="I96" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J96" s="67"/>
       <c r="K96" s="31" t="s">
@@ -12999,7 +12999,7 @@
         <v>42040003</v>
       </c>
       <c r="B97" s="92" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C97" s="8">
         <v>5</v>
@@ -13008,14 +13008,14 @@
         <v>0</v>
       </c>
       <c r="F97" s="70" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G97" s="70" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="H97" s="67"/>
       <c r="I97" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J97" s="67"/>
       <c r="K97" s="31" t="s">
@@ -13049,10 +13049,10 @@
       <c r="BD97" s="70"/>
       <c r="BE97" s="70"/>
       <c r="BU97" s="70" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="BV97" s="70" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="98" spans="1:74" x14ac:dyDescent="0.15">
@@ -13060,7 +13060,7 @@
         <v>42040004</v>
       </c>
       <c r="B98" s="92" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C98" s="8">
         <v>5</v>
@@ -13069,14 +13069,14 @@
         <v>0</v>
       </c>
       <c r="F98" s="70" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G98" s="70" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H98" s="67"/>
       <c r="I98" s="67" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J98" s="67"/>
       <c r="K98" s="31" t="s">
@@ -13110,10 +13110,10 @@
       <c r="BD98" s="70"/>
       <c r="BE98" s="70"/>
       <c r="BU98" s="70" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="BV98" s="70" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="99" spans="1:74" x14ac:dyDescent="0.15">
@@ -13158,7 +13158,7 @@
       <c r="S99" s="67"/>
       <c r="T99" s="67"/>
       <c r="U99" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V99" s="67"/>
       <c r="W99" s="23"/>
@@ -13233,7 +13233,7 @@
       <c r="S100" s="67"/>
       <c r="T100" s="67"/>
       <c r="U100" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V100" s="67"/>
       <c r="W100" s="24"/>
@@ -13377,7 +13377,7 @@
       <c r="S102" s="67"/>
       <c r="T102" s="67"/>
       <c r="U102" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V102" s="67"/>
       <c r="W102" s="24"/>
@@ -13453,7 +13453,7 @@
       <c r="S103" s="67"/>
       <c r="T103" s="67"/>
       <c r="U103" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V103" s="67"/>
       <c r="W103" s="24"/>
@@ -13607,7 +13607,7 @@
       <c r="S105" s="67"/>
       <c r="T105" s="67"/>
       <c r="U105" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V105" s="67"/>
       <c r="W105" s="24"/>
@@ -13689,7 +13689,7 @@
       <c r="S106" s="67"/>
       <c r="T106" s="67"/>
       <c r="U106" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V106" s="67"/>
       <c r="W106" s="24"/>
@@ -13770,7 +13770,7 @@
       <c r="S107" s="67"/>
       <c r="T107" s="67"/>
       <c r="U107" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V107" s="67"/>
       <c r="W107" s="24"/>
@@ -13922,7 +13922,7 @@
       <c r="S109" s="67"/>
       <c r="T109" s="67"/>
       <c r="U109" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V109" s="67"/>
       <c r="W109" s="24"/>
@@ -14008,7 +14008,7 @@
       <c r="S110" s="67"/>
       <c r="T110" s="67"/>
       <c r="U110" s="67" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="V110" s="67"/>
       <c r="W110" s="24"/>
@@ -14233,7 +14233,7 @@
         <v>1</v>
       </c>
       <c r="T113" s="99" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="U113" s="99"/>
       <c r="V113" s="99"/>
@@ -14307,7 +14307,7 @@
         <v>1</v>
       </c>
       <c r="T114" s="99" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="U114" s="99"/>
       <c r="V114" s="99"/>
@@ -14383,10 +14383,10 @@
         <v>1</v>
       </c>
       <c r="T115" s="99" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="U115" s="99" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="V115" s="99"/>
       <c r="X115" s="22"/>
@@ -14410,7 +14410,7 @@
       <c r="AU115" s="70"/>
       <c r="AV115" s="70"/>
       <c r="AZ115" s="104" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="BA115" s="8">
         <v>2</v>
@@ -14589,7 +14589,7 @@
         <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>619</v>
@@ -14712,7 +14712,7 @@
         <v>69</v>
       </c>
       <c r="AX1" s="88" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="AY1" s="88" t="s">
         <v>630</v>
@@ -14781,10 +14781,10 @@
         <v>332</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.15">
@@ -15037,7 +15037,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="80" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="J3" s="80" t="s">
         <v>621</v>
@@ -15229,10 +15229,10 @@
         <v>334</v>
       </c>
       <c r="BU3" s="80" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="BV3" s="80" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.15">
@@ -15299,7 +15299,7 @@
         <v>74</v>
       </c>
       <c r="BV4" s="70" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="5" spans="1:74" x14ac:dyDescent="0.15">
@@ -15479,7 +15479,7 @@
         <v>154</v>
       </c>
       <c r="BV7" s="69" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.15">
@@ -15534,10 +15534,10 @@
       <c r="AK8" s="60"/>
       <c r="AL8" s="60"/>
       <c r="BU8" s="66" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="BV8" s="66" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.15">
@@ -15593,10 +15593,10 @@
       <c r="AK9" s="60"/>
       <c r="AL9" s="60"/>
       <c r="BU9" s="66" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="BV9" s="66" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="10" spans="1:74" x14ac:dyDescent="0.15">
@@ -15653,10 +15653,10 @@
       <c r="BD10" s="70"/>
       <c r="BE10" s="70"/>
       <c r="BU10" s="66" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="BV10" s="66" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="11" spans="1:74" x14ac:dyDescent="0.15">
@@ -15933,7 +15933,7 @@
       <c r="U15" s="59"/>
       <c r="V15" s="59"/>
       <c r="W15" s="70" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="X15" s="59"/>
       <c r="Y15" s="60"/>
@@ -16057,7 +16057,7 @@
       <c r="U17" s="59"/>
       <c r="V17" s="59"/>
       <c r="W17" s="44" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="X17" s="59"/>
       <c r="Y17" s="60"/>
@@ -16095,7 +16095,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="70" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G18" s="44" t="s">
         <v>130</v>
@@ -16118,7 +16118,7 @@
       <c r="U18" s="59"/>
       <c r="V18" s="59"/>
       <c r="W18" s="44" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="X18" s="59"/>
       <c r="Y18" s="60"/>
@@ -16156,7 +16156,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="70" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="G19" s="44" t="s">
         <v>133</v>
@@ -16179,7 +16179,7 @@
       <c r="U19" s="59"/>
       <c r="V19" s="59"/>
       <c r="W19" s="70" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="X19" s="59"/>
       <c r="Y19" s="60"/>
@@ -16217,7 +16217,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="70" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="G20" s="44" t="s">
         <v>131</v>
@@ -16240,7 +16240,7 @@
       <c r="U20" s="59"/>
       <c r="V20" s="59"/>
       <c r="W20" s="70" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="X20" s="59"/>
       <c r="Y20" s="60"/>
@@ -16269,7 +16269,7 @@
         <v>42120011</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C21" s="58">
         <v>2</v>
@@ -16278,7 +16278,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="70" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="G21" s="44" t="s">
         <v>132</v>
@@ -16301,7 +16301,7 @@
       <c r="U21" s="59"/>
       <c r="V21" s="59"/>
       <c r="W21" s="70" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="X21" s="59"/>
       <c r="Y21" s="60"/>
@@ -16330,7 +16330,7 @@
         <v>42120012</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C22" s="58">
         <v>2</v>
@@ -16339,10 +16339,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="70" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="G22" s="70" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="H22" s="59" t="s">
         <v>11</v>
@@ -16362,7 +16362,7 @@
       <c r="U22" s="59"/>
       <c r="V22" s="59"/>
       <c r="W22" s="70" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="X22" s="59"/>
       <c r="Y22" s="60"/>
@@ -16380,10 +16380,10 @@
       <c r="AK22" s="60"/>
       <c r="AL22" s="60"/>
       <c r="BU22" s="70" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="BV22" s="70" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="23" spans="1:74" x14ac:dyDescent="0.15">
@@ -16816,7 +16816,7 @@
         <v>11</v>
       </c>
       <c r="I30" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J30" s="59"/>
       <c r="K30" s="59"/>
@@ -16881,7 +16881,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J31" s="59"/>
       <c r="K31" s="59"/>
@@ -16943,7 +16943,7 @@
         <v>11</v>
       </c>
       <c r="I32" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J32" s="59"/>
       <c r="K32" s="59"/>
@@ -17080,7 +17080,7 @@
       </c>
       <c r="H34" s="59"/>
       <c r="I34" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J34" s="67" t="s">
         <v>639</v>
@@ -17163,7 +17163,7 @@
       </c>
       <c r="H35" s="59"/>
       <c r="I35" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J35" s="67"/>
       <c r="K35" s="59"/>
@@ -17233,7 +17233,7 @@
         <v>11</v>
       </c>
       <c r="I36" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J36" s="59"/>
       <c r="K36" s="59"/>
@@ -17295,7 +17295,7 @@
         <v>11</v>
       </c>
       <c r="I37" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J37" s="59"/>
       <c r="K37" s="59"/>
@@ -17682,7 +17682,7 @@
         <v>11</v>
       </c>
       <c r="I42" s="67" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J42" s="59"/>
       <c r="K42" s="59"/>

</xml_diff>